<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@4d6217fbb3e4d20623fee1f1ab76ce8416518b58 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-location-bindings.xlsx
+++ b/StructureDefinition-us-core-location-bindings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="421">
   <si>
     <t>Property</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>extensible</t>
+  </si>
+  <si>
+    <t>☞☞☞Extensible binding inherited from FHIR R4 `Location.type`☜☜☜</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/ValueSet/us-core-location-type</t>
@@ -3591,9 +3594,11 @@
       <c r="X18" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="Y18" s="2"/>
+      <c r="Y18" t="s" s="2">
+        <v>192</v>
+      </c>
       <c r="Z18" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>75</v>
@@ -3626,7 +3631,7 @@
         <v>96</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>186</v>
@@ -3634,10 +3639,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3663,10 +3668,10 @@
         <v>164</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -3717,7 +3722,7 @@
         <v>75</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>76</v>
@@ -3740,10 +3745,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3772,7 +3777,7 @@
         <v>131</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N20" t="s" s="2">
         <v>133</v>
@@ -3813,19 +3818,19 @@
         <v>75</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AC20" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AD20" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>76</v>
@@ -3848,10 +3853,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3877,16 +3882,16 @@
         <v>157</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>75</v>
@@ -3935,7 +3940,7 @@
         <v>75</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>76</v>
@@ -3950,7 +3955,7 @@
         <v>96</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>75</v>
@@ -3958,10 +3963,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3987,10 +3992,10 @@
         <v>164</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -4041,7 +4046,7 @@
         <v>75</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>76</v>
@@ -4064,10 +4069,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4096,7 +4101,7 @@
         <v>131</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N23" t="s" s="2">
         <v>133</v>
@@ -4137,19 +4142,19 @@
         <v>75</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AC23" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AD23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>76</v>
@@ -4172,10 +4177,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4201,16 +4206,16 @@
         <v>98</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>75</v>
@@ -4259,7 +4264,7 @@
         <v>75</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>76</v>
@@ -4274,7 +4279,7 @@
         <v>96</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>75</v>
@@ -4282,10 +4287,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4311,13 +4316,13 @@
         <v>164</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -4367,7 +4372,7 @@
         <v>75</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>76</v>
@@ -4382,7 +4387,7 @@
         <v>96</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>75</v>
@@ -4390,10 +4395,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4419,14 +4424,14 @@
         <v>104</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>75</v>
@@ -4475,7 +4480,7 @@
         <v>75</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>76</v>
@@ -4490,7 +4495,7 @@
         <v>96</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>75</v>
@@ -4498,10 +4503,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4527,14 +4532,14 @@
         <v>164</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>75</v>
@@ -4583,7 +4588,7 @@
         <v>75</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>76</v>
@@ -4598,7 +4603,7 @@
         <v>96</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>75</v>
@@ -4606,10 +4611,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4632,19 +4637,19 @@
         <v>85</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>75</v>
@@ -4693,7 +4698,7 @@
         <v>75</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>76</v>
@@ -4708,7 +4713,7 @@
         <v>96</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>75</v>
@@ -4716,10 +4721,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4745,16 +4750,16 @@
         <v>164</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>75</v>
@@ -4803,7 +4808,7 @@
         <v>75</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>76</v>
@@ -4818,7 +4823,7 @@
         <v>96</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>75</v>
@@ -4826,10 +4831,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4852,13 +4857,13 @@
         <v>75</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4909,7 +4914,7 @@
         <v>75</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>76</v>
@@ -4924,7 +4929,7 @@
         <v>96</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>75</v>
@@ -4932,10 +4937,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4958,19 +4963,19 @@
         <v>75</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>75</v>
@@ -5019,7 +5024,7 @@
         <v>75</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>76</v>
@@ -5034,7 +5039,7 @@
         <v>96</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>75</v>
@@ -5042,10 +5047,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5071,10 +5076,10 @@
         <v>164</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5125,7 +5130,7 @@
         <v>75</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>76</v>
@@ -5148,10 +5153,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5180,7 +5185,7 @@
         <v>131</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N33" t="s" s="2">
         <v>133</v>
@@ -5221,19 +5226,19 @@
         <v>75</v>
       </c>
       <c r="AB33" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AC33" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AD33" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>76</v>
@@ -5256,10 +5261,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5285,16 +5290,16 @@
         <v>104</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>75</v>
@@ -5307,7 +5312,7 @@
         <v>75</v>
       </c>
       <c r="T34" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="U34" t="s" s="2">
         <v>75</v>
@@ -5322,10 +5327,10 @@
         <v>151</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Z34" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AA34" t="s" s="2">
         <v>75</v>
@@ -5343,7 +5348,7 @@
         <v>75</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>76</v>
@@ -5358,7 +5363,7 @@
         <v>96</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>75</v>
@@ -5366,10 +5371,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5395,13 +5400,13 @@
         <v>104</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5415,7 +5420,7 @@
         <v>75</v>
       </c>
       <c r="T35" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="U35" t="s" s="2">
         <v>75</v>
@@ -5430,10 +5435,10 @@
         <v>151</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>75</v>
@@ -5451,7 +5456,7 @@
         <v>75</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>76</v>
@@ -5466,7 +5471,7 @@
         <v>96</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>75</v>
@@ -5474,10 +5479,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5503,16 +5508,16 @@
         <v>164</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>75</v>
@@ -5525,7 +5530,7 @@
         <v>75</v>
       </c>
       <c r="T36" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="U36" t="s" s="2">
         <v>75</v>
@@ -5561,7 +5566,7 @@
         <v>75</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>76</v>
@@ -5576,7 +5581,7 @@
         <v>96</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>75</v>
@@ -5584,10 +5589,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5613,10 +5618,10 @@
         <v>164</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5631,7 +5636,7 @@
         <v>75</v>
       </c>
       <c r="T37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="U37" t="s" s="2">
         <v>75</v>
@@ -5667,7 +5672,7 @@
         <v>75</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>76</v>
@@ -5682,7 +5687,7 @@
         <v>96</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>75</v>
@@ -5690,14 +5695,14 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
@@ -5719,10 +5724,10 @@
         <v>164</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -5737,7 +5742,7 @@
         <v>75</v>
       </c>
       <c r="T38" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="U38" t="s" s="2">
         <v>75</v>
@@ -5773,7 +5778,7 @@
         <v>75</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>76</v>
@@ -5788,7 +5793,7 @@
         <v>96</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>75</v>
@@ -5796,14 +5801,14 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -5825,13 +5830,13 @@
         <v>164</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -5845,7 +5850,7 @@
         <v>75</v>
       </c>
       <c r="T39" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="U39" t="s" s="2">
         <v>75</v>
@@ -5881,7 +5886,7 @@
         <v>75</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>76</v>
@@ -5896,7 +5901,7 @@
         <v>96</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>75</v>
@@ -5904,14 +5909,14 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -5933,10 +5938,10 @@
         <v>164</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5951,7 +5956,7 @@
         <v>75</v>
       </c>
       <c r="T40" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="U40" t="s" s="2">
         <v>75</v>
@@ -5966,10 +5971,10 @@
         <v>191</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>75</v>
@@ -5987,7 +5992,7 @@
         <v>75</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>76</v>
@@ -6002,7 +6007,7 @@
         <v>96</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>75</v>
@@ -6010,14 +6015,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6039,10 +6044,10 @@
         <v>164</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6057,7 +6062,7 @@
         <v>75</v>
       </c>
       <c r="T41" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="U41" t="s" s="2">
         <v>75</v>
@@ -6093,7 +6098,7 @@
         <v>75</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>76</v>
@@ -6108,7 +6113,7 @@
         <v>96</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>75</v>
@@ -6116,10 +6121,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6145,13 +6150,13 @@
         <v>164</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6201,7 +6206,7 @@
         <v>75</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>76</v>
@@ -6216,7 +6221,7 @@
         <v>96</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>75</v>
@@ -6224,10 +6229,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6250,17 +6255,17 @@
         <v>85</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>75</v>
@@ -6273,7 +6278,7 @@
         <v>75</v>
       </c>
       <c r="T43" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="U43" t="s" s="2">
         <v>75</v>
@@ -6309,7 +6314,7 @@
         <v>75</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>76</v>
@@ -6324,7 +6329,7 @@
         <v>96</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>75</v>
@@ -6332,10 +6337,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6361,14 +6366,14 @@
         <v>188</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>75</v>
@@ -6393,13 +6398,13 @@
         <v>75</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>75</v>
@@ -6417,7 +6422,7 @@
         <v>75</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>76</v>
@@ -6432,7 +6437,7 @@
         <v>96</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>186</v>
@@ -6440,10 +6445,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6466,17 +6471,17 @@
         <v>75</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="P45" t="s" s="2">
         <v>75</v>
@@ -6525,7 +6530,7 @@
         <v>75</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>76</v>
@@ -6540,7 +6545,7 @@
         <v>96</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>75</v>
@@ -6548,10 +6553,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6577,10 +6582,10 @@
         <v>164</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -6631,7 +6636,7 @@
         <v>75</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>76</v>
@@ -6654,10 +6659,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6686,7 +6691,7 @@
         <v>131</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>133</v>
@@ -6739,7 +6744,7 @@
         <v>75</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>76</v>
@@ -6762,14 +6767,14 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
@@ -6791,10 +6796,10 @@
         <v>130</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N48" t="s" s="2">
         <v>133</v>
@@ -6849,7 +6854,7 @@
         <v>75</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>76</v>
@@ -6872,10 +6877,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -6898,13 +6903,13 @@
         <v>75</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -6955,7 +6960,7 @@
         <v>75</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>84</v>
@@ -6970,7 +6975,7 @@
         <v>96</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>75</v>
@@ -6978,10 +6983,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7004,13 +7009,13 @@
         <v>75</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7061,7 +7066,7 @@
         <v>75</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>84</v>
@@ -7076,7 +7081,7 @@
         <v>96</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>75</v>
@@ -7084,10 +7089,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7110,13 +7115,13 @@
         <v>75</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7167,7 +7172,7 @@
         <v>75</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>76</v>
@@ -7182,7 +7187,7 @@
         <v>96</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>75</v>
@@ -7190,10 +7195,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7216,19 +7221,19 @@
         <v>85</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="O52" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>75</v>
@@ -7277,7 +7282,7 @@
         <v>75</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>76</v>
@@ -7292,7 +7297,7 @@
         <v>96</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>75</v>
@@ -7300,10 +7305,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7326,17 +7331,17 @@
         <v>75</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="P53" t="s" s="2">
         <v>75</v>
@@ -7385,7 +7390,7 @@
         <v>75</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>76</v>
@@ -7400,7 +7405,7 @@
         <v>96</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>75</v>
@@ -7408,10 +7413,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7434,16 +7439,16 @@
         <v>75</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -7493,7 +7498,7 @@
         <v>75</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>76</v>
@@ -7508,7 +7513,7 @@
         <v>96</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>75</v>
@@ -7516,10 +7521,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -7545,10 +7550,10 @@
         <v>164</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -7599,7 +7604,7 @@
         <v>75</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>76</v>
@@ -7622,10 +7627,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -7654,7 +7659,7 @@
         <v>131</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N56" t="s" s="2">
         <v>133</v>
@@ -7707,7 +7712,7 @@
         <v>75</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>76</v>
@@ -7730,14 +7735,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -7759,10 +7764,10 @@
         <v>130</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N57" t="s" s="2">
         <v>133</v>
@@ -7817,7 +7822,7 @@
         <v>75</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>76</v>
@@ -7840,10 +7845,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -7869,10 +7874,10 @@
         <v>104</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -7902,10 +7907,10 @@
         <v>151</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="Z58" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>75</v>
@@ -7923,7 +7928,7 @@
         <v>75</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>76</v>
@@ -7938,7 +7943,7 @@
         <v>96</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>75</v>
@@ -7946,10 +7951,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -7972,13 +7977,13 @@
         <v>75</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8029,7 +8034,7 @@
         <v>75</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>76</v>
@@ -8044,7 +8049,7 @@
         <v>96</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>75</v>
@@ -8052,10 +8057,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8078,13 +8083,13 @@
         <v>75</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8135,7 +8140,7 @@
         <v>75</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>76</v>
@@ -8150,7 +8155,7 @@
         <v>96</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>75</v>
@@ -8158,10 +8163,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8184,13 +8189,13 @@
         <v>75</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8241,7 +8246,7 @@
         <v>75</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>76</v>
@@ -8256,7 +8261,7 @@
         <v>96</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>75</v>
@@ -8264,10 +8269,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8293,10 +8298,10 @@
         <v>164</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -8347,7 +8352,7 @@
         <v>75</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>76</v>
@@ -8370,10 +8375,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -8396,17 +8401,17 @@
         <v>75</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="P63" t="s" s="2">
         <v>75</v>
@@ -8455,7 +8460,7 @@
         <v>75</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>76</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@ed4b12802d69a3251607d7adb77158c693d12635 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-location-bindings.xlsx
+++ b/StructureDefinition-us-core-location-bindings.xlsx
@@ -617,7 +617,7 @@
     <t>☞☞☞Extensible binding inherited from FHIR R4 `Location.type`☜☜☜</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-location-type</t>
+    <t>http://terminology.hl7.org/ValueSet/v3-ServiceDeliveryLocationRoleType</t>
   </si>
   <si>
     <t>.code</t>
@@ -1675,7 +1675,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="84.6796875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="53.078125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="67.80078125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>